<commit_message>
almos tready for second round
</commit_message>
<xml_diff>
--- a/covid/alburez_budget.xlsx
+++ b/covid/alburez_budget.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Position</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>Please detail each cost position on the left regarding the quantity, the item, and with positions also the salary grade. On the right please enter the required amount for the total duration (after subtraction of own contributions, incl. VAT, if applicable). In cooperative projects it is often dispensable to fill-in a separate budget form for each co-applicant. For some funding initiatives the respective ‘Information for Applicants’ regulates the break-down of costs. Please agree in advance which budget items are considered by the principal investigator.</t>
+  </si>
+  <si>
+    <t>One Research Assistant to work on methodological development (1 year)</t>
+  </si>
+  <si>
+    <t>One PhD student to conduct empirical research (18 months)</t>
+  </si>
+  <si>
+    <t>Travel to conferences and workshops for PI and research assistant. Potential visit to the Demography Unit of Stockholm University (Sweden) to work on micro-level data</t>
+  </si>
+  <si>
+    <t>Article processing and open access charges (expected a minimum of three publications in top journals)</t>
   </si>
 </sst>
 </file>
@@ -92,7 +104,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -100,6 +112,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -402,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -446,35 +461,80 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>23000</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>67500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>6000</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f>SUM(C5:C12)</f>
+        <v>103500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>